<commit_message>
handle the problem of key words
</commit_message>
<xml_diff>
--- a/sometest.xlsx
+++ b/sometest.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>64231191_刘袆曼</t>
   </si>
@@ -36,6 +36,74 @@
   </si>
   <si>
     <t>关于参考文献的交叉引用，文章中没有对参考文献的引用，所以。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12061049_谢何涛_学生成绩相关性分析与系统设计实现.docx</t>
+  </si>
+  <si>
+    <t>这篇修改之后没什么问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关键词部分目前还没想好</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关于封面的单位代码的缩进有一些问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12061053-李子靓-面向产品评论的情感要素抽取及情感倾向性分析(3).docx</t>
+  </si>
+  <si>
+    <t>左侧缩进还未修改</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>段首有Tab还未决定需要改否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1145黄强_毕业论文.docx</t>
+  </si>
+  <si>
+    <t>摘要字体未改正，发现rFonts标签中含有一eastAsiaTheme标签，即文章中使用主题字体</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部分地方含有左侧缩进和悬挂缩进</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tab键目前未消</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>目录地方第三级目录标题采用了(1)检测为一级目录标题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二稿-62231365-钟华-二班-智能手机邮件收发的研究与实现(Android).docx</t>
+  </si>
+  <si>
+    <t>英文摘要部分顺序不对导致定位错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部分地方有右侧缩进与左侧缩进</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关于列表项的编号的字体样式存在于number.xml文件中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>关键词还未改正</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文本框</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -385,19 +453,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="73.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -405,24 +473,106 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="B26" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>